<commit_message>
Added final rf plots and updated the code to run smoothly. All plots have been run, except for MDS plot
</commit_message>
<xml_diff>
--- a/data/Predictions/analysis_rf_predictions_best_genes.xlsx
+++ b/data/Predictions/analysis_rf_predictions_best_genes.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -494,10 +494,10 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.8794871794871788</v>
+        <v>0.8769230769230763</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9562130177514788</v>
+        <v>0.9548980933596314</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -529,10 +529,10 @@
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>0.8564102564102557</v>
+        <v>0.8615384615384606</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9555555555555552</v>
+        <v>0.9539776462853382</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -564,19 +564,19 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.8564102564102558</v>
+        <v>0.8743589743589736</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9544378698224849</v>
+        <v>0.97120315581854</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000204387, ENSG00000215908, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000204387, ENSG00000233493, ENSG00000215908</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, C6orf48, CROCCP2, DPM3</t>
+          <t>SNHG5, SNHG8, C6orf48, TMEM238, CROCCP2</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -599,19 +599,19 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>0.871794871794871</v>
+        <v>0.8923076923076918</v>
       </c>
       <c r="G5" t="n">
-        <v>0.965023011176857</v>
+        <v>0.9697567389875081</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000204387, ENSG00000215908, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000258920, ENSG00000204387, ENSG00000215908</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RN7SL2, C6orf48, CROCCP2, DPM3</t>
+          <t>SNHG5, SNHG8, RN7SL2, FOXN3-AS1, C6orf48, CROCCP2</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -634,19 +634,19 @@
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>0.8615384615384608</v>
+        <v>0.8999999999999997</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9608152531229452</v>
+        <v>0.9760683760683755</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000204387, ENSG00000215908, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000258920, ENSG00000204387, ENSG00000233493, ENSG00000215908</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, C6orf48, CROCCP2, DPM3</t>
+          <t>SNHG5, SNHG8, RN7SL2, FOXN3-AS1, C6orf48, TMEM238, CROCCP2</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -669,19 +669,19 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.8948717948717944</v>
+        <v>0.871794871794871</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9718606180144638</v>
+        <v>0.9584483892176197</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000258920, ENSG00000204387, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RN7SL2, C6orf48, TMEM238, CROCCP2, GAS5, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, FOXN3-AS1, C6orf48, CROCCP2, GAS5, DPM3</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -704,19 +704,19 @@
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>0.8794871794871788</v>
+        <v>0.8846153846153839</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9690992767915843</v>
+        <v>0.9742274819197891</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000255559, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RN7SL2, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, ZNF252P-AS1, C6orf48, TMEM238, CROCCP2, GAS5</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -739,19 +739,19 @@
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.8794871794871788</v>
+        <v>0.8871794871794867</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9673898750821823</v>
+        <v>0.9733070348454961</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000258920, ENSG00000225864, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5</t>
+          <t>SNHG5, SNHG8, RN7SL2, FOXN3-AS1, HCG4P11, C6orf48, TMEM238, CROCCP2, GAS5, DPM3</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -774,19 +774,19 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>0.8666666666666657</v>
+        <v>0.8846153846153839</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9656804733727806</v>
+        <v>0.9642340565417487</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000215908, ENSG00000215414, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000179085</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, CROCCP2, PSMA6P1, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, TMEM191A, C6orf48, TMEM238, CROCCP2, DPM3</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -809,19 +809,19 @@
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.8923076923076918</v>
+        <v>0.8794871794871788</v>
       </c>
       <c r="G11" t="n">
-        <v>0.969625246548323</v>
+        <v>0.9654832347140034</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000255559, ENSG00000225864, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000230979, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000272906, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000215414, ENSG00000230979</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, ZNF252P-AS1, HCG4P11, C6orf48, TMEM238, CROCCP2, GAS5, AC079250.1, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, RP11-533E19.7, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, PSMA6P1, AC079250.1</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -844,19 +844,19 @@
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.8846153846153841</v>
+        <v>0.8846153846153839</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9701512163050621</v>
+        <v>0.9679158448389215</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000230979, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, AC079250.1, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, DPM3</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -879,19 +879,19 @@
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.8846153846153841</v>
+        <v>0.8871794871794865</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9685733070348451</v>
+        <v>0.9671268902038129</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000230979, ENSG00000179085</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, AC079250.1, DPM3</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -914,19 +914,19 @@
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>0.9025641025641022</v>
+        <v>0.8871794871794865</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9723865877712028</v>
+        <v>0.9708086785009856</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000224066, ENSG00000230979, ENSG00000253683, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000179085</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, RP4-622L5.7, AC079250.1, CTB-79E8.3, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, DPM3</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -952,16 +952,16 @@
         <v>0.8846153846153839</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9702827087442468</v>
+        <v>0.9693622616699532</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000215414, ENSG00000230979, ENSG00000179085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000224066, ENSG00000215414, ENSG00000253683, ENSG00000179085</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, PSMA6P1, AC079250.1, DPM3</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, RP4-622L5.7, PSMA6P1, CTB-79E8.3, DPM3</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -984,19 +984,19 @@
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>0.8948717948717944</v>
+        <v>0.902564102564102</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9718606180144638</v>
+        <v>0.9729783037475344</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000274012, ENSG00000278771, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000215414, ENSG00000230979, ENSG00000253683, ENSG00000179085, ENSG00000226085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000224066, ENSG00000253683, ENSG00000179085</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RN7SL2, Metazoa_SRP, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, PSMA6P1, AC079250.1, CTB-79E8.3, DPM3, UQCRFS1P1</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, RP4-622L5.7, CTB-79E8.3, DPM3</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1019,19 +1019,19 @@
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>0.8999999999999997</v>
+        <v>0.8897435897435892</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9702827087442463</v>
+        <v>0.9705456936226163</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000215414, ENSG00000230979, ENSG00000179085, ENSG00000226085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000224066, ENSG00000215414, ENSG00000230979, ENSG00000179085</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, PSMA6P1, AC079250.1, DPM3, UQCRFS1P1</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, RP4-622L5.7, PSMA6P1, AC079250.1, DPM3</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1054,19 +1054,19 @@
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>0.8923076923076918</v>
+        <v>0.8974358974358971</v>
       </c>
       <c r="G18" t="n">
-        <v>0.970808678500986</v>
+        <v>0.9722550953320178</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000224066, ENSG00000215414, ENSG00000253683, ENSG00000179085, ENSG00000226085</t>
+          <t>ENSG00000203875, ENSG00000269893, ENSG00000236552, ENSG00000274012, ENSG00000278771, ENSG00000272906, ENSG00000255559, ENSG00000258920, ENSG00000225864, ENSG00000226287, ENSG00000204387, ENSG00000233493, ENSG00000215908, ENSG00000234741, ENSG00000215414, ENSG00000230979, ENSG00000253683, ENSG00000179085, ENSG00000226085</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, RP4-622L5.7, PSMA6P1, CTB-79E8.3, DPM3, UQCRFS1P1</t>
+          <t>SNHG5, SNHG8, RPL13AP5, RN7SL2, Metazoa_SRP, RP11-533E19.7, ZNF252P-AS1, FOXN3-AS1, HCG4P11, TMEM191A, C6orf48, TMEM238, CROCCP2, GAS5, PSMA6P1, AC079250.1, CTB-79E8.3, DPM3, UQCRFS1P1</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Subset</t>
+          <t>SUBSET</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1089,10 +1089,10 @@
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.8897435897435892</v>
+        <v>0.8974358974358971</v>
       </c>
       <c r="G19" t="n">
-        <v>0.971071663379355</v>
+        <v>0.9725180802103874</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>

</xml_diff>